<commit_message>
update data to present day
</commit_message>
<xml_diff>
--- a/data/Wordle Group Results.xlsx
+++ b/data/Wordle Group Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brianspencer/Documents/GitHub/wordle/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4D9B9E1-FD60-A940-8E49-E869764B05A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C840D03-463B-6849-81AF-D8D0D8E701BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20780" tabRatio="642" activeTab="1" xr2:uid="{9CF507EB-1BFD-487F-B619-C1323D8E19B5}"/>
+    <workbookView xWindow="-20" yWindow="500" windowWidth="35840" windowHeight="20780" tabRatio="642" activeTab="1" xr2:uid="{9CF507EB-1BFD-487F-B619-C1323D8E19B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2327" uniqueCount="743">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2335" uniqueCount="746">
   <si>
     <t>Date</t>
   </si>
@@ -2267,6 +2267,15 @@
   </si>
   <si>
     <t>Choir</t>
+  </si>
+  <si>
+    <t>Blend</t>
+  </si>
+  <si>
+    <t>Peace</t>
+  </si>
+  <si>
+    <t>Write</t>
   </si>
 </sst>
 </file>
@@ -2487,10 +2496,10 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5569,8 +5578,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{D691CA6C-2060-43BD-B6D0-81E79FA5F211}" name="Season4Data" displayName="Season4Data" ref="A1:U66" totalsRowShown="0" headerRowDxfId="134" dataDxfId="132" headerRowBorderDxfId="133" tableBorderDxfId="131">
-  <autoFilter ref="A1:U66" xr:uid="{5EF9BA9D-CFC1-43C8-9987-E2F4970F881B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{D691CA6C-2060-43BD-B6D0-81E79FA5F211}" name="Season4Data" displayName="Season4Data" ref="A1:U68" totalsRowShown="0" headerRowDxfId="134" dataDxfId="132" headerRowBorderDxfId="133" tableBorderDxfId="131">
+  <autoFilter ref="A1:U68" xr:uid="{5EF9BA9D-CFC1-43C8-9987-E2F4970F881B}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U61">
     <sortCondition ref="A1:A61"/>
   </sortState>
@@ -7231,11 +7240,11 @@
       </c>
       <c r="B41">
         <f>COUNTIF(Season4Data[Winner],Season4Overall[[#This Row],[Person:]])</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D41">
         <f>SUMPRODUCT(--(Season4Data[Winner]=Season4Overall[[#This Row],[Person:]]),--(Season4Data[Tiebreakers]))</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E41">
         <f>SUMPRODUCT(--(Season4Data[Winner]=Season4Overall[[#This Row],[Person:]]),--(Season4Data[Tiebreakers]=FALSE))</f>
@@ -7243,11 +7252,11 @@
       </c>
       <c r="F41">
         <f>Season4Overall[[#This Row],[Solo]]/COUNTIF(Season4Data[Brian],"&lt;&gt;"&amp;"")*100</f>
-        <v>20.3125</v>
+        <v>21.212121212121211</v>
       </c>
       <c r="G41" s="1">
         <f t="array" ref="G41">MAX(IF(Season4Data[Winner]=Season4Overall[[#This Row],[Person:]],Season4Data[Date]))</f>
-        <v>45164</v>
+        <v>45166</v>
       </c>
       <c r="H41">
         <f t="array" ref="H41">DATEDIF(Season4Overall[[#This Row],[Last Win]],MAX(Season4Data[Date]),"d")</f>
@@ -7263,15 +7272,15 @@
       </c>
       <c r="M41">
         <f>AVERAGE(Season4Data[Brian])</f>
-        <v>4</v>
+        <v>4.0151515151515156</v>
       </c>
       <c r="O41">
         <f>AVERAGEIF(Season4Data[Word Picker],Season4Overall[[#This Row],[Person:]],Season4Data[Remaining Words])</f>
-        <v>812.58333333333337</v>
+        <v>911.69230769230774</v>
       </c>
       <c r="P41">
         <f>AVERAGEIF(Season4Data[Word Picker],Season4Overall[[#This Row],[Person:]],Season4Data[Average Guess])</f>
-        <v>3.700396825396826</v>
+        <v>3.7849816849816853</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.2">
@@ -7300,7 +7309,7 @@
       </c>
       <c r="H42">
         <f t="array" ref="H42">DATEDIF(Season4Overall[[#This Row],[Last Win]],MAX(Season4Data[Date]),"d")</f>
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J42">
         <f>SUMPRODUCT(--(Season4Data[Best Guess]=Season4Data[Elisabeth]))-COUNTIF(Season4Data[Winner],Season4Overall[[#This Row],[Person:]])</f>
@@ -7329,7 +7338,7 @@
       </c>
       <c r="B43">
         <f>COUNTIF(Season4Data[Winner],Season4Overall[[#This Row],[Person:]])</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D43">
         <f>SUMPRODUCT(--(Season4Data[Winner]=Season4Overall[[#This Row],[Person:]]),--(Season4Data[Tiebreakers]))</f>
@@ -7337,23 +7346,23 @@
       </c>
       <c r="E43">
         <f>SUMPRODUCT(--(Season4Data[Winner]=Season4Overall[[#This Row],[Person:]]),--(Season4Data[Tiebreakers]=FALSE))</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F43">
         <f>Season4Overall[[#This Row],[Solo]]/COUNTIF(Season4Data[Kendall],"&lt;&gt;"&amp;"")*100</f>
-        <v>12.307692307692308</v>
+        <v>13.432835820895523</v>
       </c>
       <c r="G43" s="1">
         <f t="array" ref="G43">MAX(IF(Season4Data[Winner]=Season4Overall[[#This Row],[Person:]],Season4Data[Date]))</f>
-        <v>45158</v>
+        <v>45165</v>
       </c>
       <c r="H43">
         <f t="array" ref="H43">DATEDIF(Season4Overall[[#This Row],[Last Win]],MAX(Season4Data[Date]),"d")</f>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="J43">
         <f>SUMPRODUCT(--(Season4Data[Best Guess]=Season4Data[Kendall]))-COUNTIF(Season4Data[Winner],Season4Overall[[#This Row],[Person:]])</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L43">
         <f>MIN(Season4Data[Kendall])</f>
@@ -7361,15 +7370,15 @@
       </c>
       <c r="M43">
         <f>AVERAGE(Season4Data[Kendall])</f>
-        <v>4.0615384615384613</v>
+        <v>4.0298507462686564</v>
       </c>
       <c r="O43">
         <f>AVERAGEIF(Season4Data[Word Picker],Season4Overall[[#This Row],[Person:]],Season4Data[Remaining Words])</f>
-        <v>1747.625</v>
+        <v>1569.2222222222222</v>
       </c>
       <c r="P43">
         <f>AVERAGEIF(Season4Data[Word Picker],Season4Overall[[#This Row],[Person:]],Season4Data[Average Guess])</f>
-        <v>4.020833333333333</v>
+        <v>4</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.2">
@@ -7390,7 +7399,7 @@
       </c>
       <c r="F44">
         <f>Season4Overall[[#This Row],[Solo]]/COUNTIF(Season4Data[Kimball],"&lt;&gt;"&amp;"")*100</f>
-        <v>9.2307692307692317</v>
+        <v>8.9552238805970141</v>
       </c>
       <c r="G44" s="1">
         <f t="array" ref="G44">MAX(IF(Season4Data[Winner]=Season4Overall[[#This Row],[Person:]],Season4Data[Date]))</f>
@@ -7398,7 +7407,7 @@
       </c>
       <c r="H44">
         <f t="array" ref="H44">DATEDIF(Season4Overall[[#This Row],[Last Win]],MAX(Season4Data[Date]),"d")</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J44">
         <f>SUMPRODUCT(--(Season4Data[Best Guess]=Season4Data[Kimball]))-COUNTIF(Season4Data[Winner],Season4Overall[[#This Row],[Person:]])</f>
@@ -7410,7 +7419,7 @@
       </c>
       <c r="M44">
         <f>AVERAGE(Season4Data[Kimball])</f>
-        <v>4.0615384615384613</v>
+        <v>4.0746268656716422</v>
       </c>
       <c r="O44">
         <f>AVERAGEIF(Season4Data[Word Picker],Season4Overall[[#This Row],[Person:]],Season4Data[Remaining Words])</f>
@@ -7439,7 +7448,7 @@
       </c>
       <c r="F45">
         <f>Season4Overall[[#This Row],[Solo]]/COUNTIF(Season4Data[Lee Ann],"&lt;&gt;"&amp;"")*100</f>
-        <v>15.384615384615385</v>
+        <v>14.925373134328357</v>
       </c>
       <c r="G45" s="1">
         <f t="array" ref="G45">MAX(IF(Season4Data[Winner]=Season4Overall[[#This Row],[Person:]],Season4Data[Date]))</f>
@@ -7447,11 +7456,11 @@
       </c>
       <c r="H45">
         <f t="array" ref="H45">DATEDIF(Season4Overall[[#This Row],[Last Win]],MAX(Season4Data[Date]),"d")</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J45">
         <f>SUMPRODUCT(--(Season4Data[Best Guess]=Season4Data[Lee Ann]))-COUNTIF(Season4Data[Winner],Season4Overall[[#This Row],[Person:]])</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="L45">
         <f>MIN(Season4Data[Lee Ann])</f>
@@ -7459,7 +7468,7 @@
       </c>
       <c r="M45">
         <f>AVERAGE(Season4Data[Lee Ann])</f>
-        <v>4.0615384615384613</v>
+        <v>4.0597014925373136</v>
       </c>
       <c r="O45">
         <f>AVERAGEIF(Season4Data[Word Picker],Season4Overall[[#This Row],[Person:]],Season4Data[Remaining Words])</f>
@@ -7488,7 +7497,7 @@
       </c>
       <c r="F46">
         <f>Season4Overall[[#This Row],[Solo]]/COUNTIF(Season4Data[Sam],"&lt;&gt;"&amp;"")*100</f>
-        <v>16.666666666666664</v>
+        <v>16.393442622950818</v>
       </c>
       <c r="G46" s="1">
         <f t="array" ref="G46">MAX(IF(Season4Data[Winner]=Season4Overall[[#This Row],[Person:]],Season4Data[Date]))</f>
@@ -7496,7 +7505,7 @@
       </c>
       <c r="H46">
         <f t="array" ref="H46">DATEDIF(Season4Overall[[#This Row],[Last Win]],MAX(Season4Data[Date]),"d")</f>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J46">
         <f>SUMPRODUCT(--(Season4Data[Best Guess]=Season4Data[Sam]))-(COUNTIF(Season4Data[Winner],Season4Overall[[#This Row],[Person:]]))</f>
@@ -7508,7 +7517,7 @@
       </c>
       <c r="M46">
         <f>AVERAGE(Season4Data[Sam])</f>
-        <v>4.0166666666666666</v>
+        <v>4.0163934426229506</v>
       </c>
       <c r="O46">
         <f>AVERAGEIF(Season4Data[Word Picker],Season4Overall[[#This Row],[Person:]],Season4Data[Remaining Words])</f>
@@ -7537,7 +7546,7 @@
       </c>
       <c r="F47">
         <f>Season4Overall[[#This Row],[Solo]]/COUNTIF(Season4Data[Spencer],"&lt;&gt;"&amp;"")*100</f>
-        <v>23.4375</v>
+        <v>22.727272727272727</v>
       </c>
       <c r="G47" s="1">
         <f t="array" ref="G47">MAX(IF(Season4Data[Winner]=Season4Overall[[#This Row],[Person:]],Season4Data[Date]))</f>
@@ -7545,7 +7554,7 @@
       </c>
       <c r="H47">
         <f t="array" ref="H47">DATEDIF(Season4Overall[[#This Row],[Last Win]],MAX(Season4Data[Date]),"d")</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J47">
         <f>SUMPRODUCT(--(Season4Data[Best Guess]=Season4Data[Spencer]))-(COUNTIF(Season4Data[Winner],Season4Overall[[#This Row],[Person:]]))</f>
@@ -7557,7 +7566,7 @@
       </c>
       <c r="M47">
         <f>AVERAGE(Season4Data[Spencer])</f>
-        <v>3.90625</v>
+        <v>3.9545454545454546</v>
       </c>
       <c r="O47">
         <f>AVERAGEIF(Season4Data[Word Picker],Season4Overall[[#This Row],[Person:]],Season4Data[Remaining Words])</f>
@@ -7574,23 +7583,23 @@
       </c>
       <c r="B48">
         <f>AVERAGE(B41:B47)</f>
-        <v>9.2857142857142865</v>
+        <v>9.5714285714285712</v>
       </c>
       <c r="D48">
         <f>AVERAGE(D41:D47)</f>
-        <v>4.7142857142857144</v>
+        <v>4.8571428571428568</v>
       </c>
       <c r="E48">
         <f>AVERAGE(E41:E47)</f>
-        <v>4.5714285714285712</v>
+        <v>4.7142857142857144</v>
       </c>
       <c r="F48">
         <f>AVERAGE(Season4Overall[Win Percentage])</f>
-        <v>15.436289900575616</v>
+        <v>15.480079301778764</v>
       </c>
       <c r="J48">
         <f>AVERAGE(J41:J47)</f>
-        <v>12.571428571428571</v>
+        <v>12.857142857142858</v>
       </c>
       <c r="L48">
         <f>AVERAGE(L41:L47)</f>
@@ -7598,15 +7607,15 @@
       </c>
       <c r="M48">
         <f>AVERAGE(M41:M47)</f>
-        <v>4.0408719256933541</v>
+        <v>4.0469772779098516</v>
       </c>
       <c r="O48">
         <f>AVERAGE(Season4Data[Remaining Words])</f>
-        <v>1169.2461538461539</v>
+        <v>1167.8208955223881</v>
       </c>
       <c r="P48">
         <f>AVERAGE(Season4Data[Average Guess])</f>
-        <v>4.0226373626373624</v>
+        <v>4.03141435678749</v>
       </c>
     </row>
   </sheetData>
@@ -7629,8 +7638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{697A79C7-C0D8-4420-B173-FCD3997E5B91}">
   <dimension ref="A1:AA115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11323,59 +11332,55 @@
       <c r="A62" s="1">
         <v>45160</v>
       </c>
-      <c r="B62" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="C62" s="31" t="s">
+      <c r="B62" t="s">
+        <v>4</v>
+      </c>
+      <c r="C62" t="s">
         <v>735</v>
       </c>
-      <c r="D62" s="31" t="s">
+      <c r="D62" t="s">
         <v>736</v>
       </c>
-      <c r="E62" s="31" t="s">
+      <c r="E62" t="s">
         <v>11</v>
       </c>
-      <c r="F62" s="31">
-        <v>1</v>
-      </c>
-      <c r="G62" s="31"/>
-      <c r="H62" s="34">
+      <c r="F62">
+        <v>1</v>
+      </c>
+      <c r="H62" s="31">
         <v>2686</v>
       </c>
-      <c r="I62" s="31"/>
-      <c r="J62" s="31"/>
-      <c r="K62" s="32">
+      <c r="K62" s="15">
         <f>MIN(Season4Data[[#This Row],[Brian]:[Spencer]])</f>
         <v>3</v>
       </c>
-      <c r="L62" s="33">
+      <c r="L62" s="29">
         <f>AVERAGE(Season4Data[[#This Row],[Brian]:[Spencer]])</f>
         <v>3.7142857142857144</v>
       </c>
-      <c r="M62" s="31" t="b">
+      <c r="M62" t="b">
         <f>IF(COUNTIF(Season4Data[[#This Row],[Brian]:[Spencer]], Season3Data[[#This Row],[Best Guess]]) &gt; 1, TRUE, FALSE)</f>
         <v>1</v>
       </c>
-      <c r="N62" s="31"/>
-      <c r="O62" s="31">
-        <v>4</v>
-      </c>
-      <c r="P62" s="31">
-        <v>4</v>
-      </c>
-      <c r="Q62" s="31">
-        <v>4</v>
-      </c>
-      <c r="R62" s="31">
-        <v>3</v>
-      </c>
-      <c r="S62" s="31">
-        <v>3</v>
-      </c>
-      <c r="T62" s="31">
-        <v>4</v>
-      </c>
-      <c r="U62" s="31">
+      <c r="O62">
+        <v>4</v>
+      </c>
+      <c r="P62">
+        <v>4</v>
+      </c>
+      <c r="Q62">
+        <v>4</v>
+      </c>
+      <c r="R62">
+        <v>3</v>
+      </c>
+      <c r="S62">
+        <v>3</v>
+      </c>
+      <c r="T62">
+        <v>4</v>
+      </c>
+      <c r="U62">
         <v>4</v>
       </c>
       <c r="X62" t="s">
@@ -11389,57 +11394,52 @@
       <c r="A63" s="1">
         <v>45161</v>
       </c>
-      <c r="B63" s="31" t="s">
+      <c r="B63" t="s">
         <v>11</v>
       </c>
-      <c r="C63" s="31" t="s">
+      <c r="C63" t="s">
         <v>737</v>
       </c>
-      <c r="D63" s="31" t="s">
+      <c r="D63" t="s">
         <v>738</v>
       </c>
-      <c r="E63" s="31" t="s">
+      <c r="E63" t="s">
         <v>13</v>
       </c>
-      <c r="F63" s="31">
-        <v>1</v>
-      </c>
-      <c r="G63" s="31"/>
-      <c r="H63" s="31">
+      <c r="F63">
+        <v>1</v>
+      </c>
+      <c r="H63">
         <v>2991</v>
       </c>
-      <c r="I63" s="31"/>
-      <c r="J63" s="31"/>
-      <c r="K63" s="32">
+      <c r="K63" s="15">
         <f>MIN(Season4Data[[#This Row],[Brian]:[Spencer]])</f>
         <v>4</v>
       </c>
-      <c r="L63" s="33">
+      <c r="L63" s="29">
         <f>AVERAGE(Season4Data[[#This Row],[Brian]:[Spencer]])</f>
         <v>4.833333333333333</v>
       </c>
-      <c r="M63" s="31" t="b">
+      <c r="M63" t="b">
         <f>IF(COUNTIF(Season4Data[[#This Row],[Brian]:[Spencer]], Season3Data[[#This Row],[Best Guess]]) &gt; 1, TRUE, FALSE)</f>
         <v>0</v>
       </c>
-      <c r="N63" s="31"/>
-      <c r="O63" s="31">
-        <v>5</v>
-      </c>
-      <c r="P63" s="31"/>
-      <c r="Q63" s="31">
-        <v>5</v>
-      </c>
-      <c r="R63" s="31">
-        <v>4</v>
-      </c>
-      <c r="S63" s="31">
-        <v>4</v>
-      </c>
-      <c r="T63" s="31">
-        <v>6</v>
-      </c>
-      <c r="U63" s="31">
+      <c r="O63">
+        <v>5</v>
+      </c>
+      <c r="Q63">
+        <v>5</v>
+      </c>
+      <c r="R63">
+        <v>4</v>
+      </c>
+      <c r="S63">
+        <v>4</v>
+      </c>
+      <c r="T63">
+        <v>6</v>
+      </c>
+      <c r="U63">
         <v>5</v>
       </c>
       <c r="X63" t="s">
@@ -11453,57 +11453,52 @@
       <c r="A64" s="1">
         <v>45162</v>
       </c>
-      <c r="B64" s="31" t="s">
+      <c r="B64" t="s">
         <v>13</v>
       </c>
-      <c r="C64" s="31" t="s">
+      <c r="C64" t="s">
         <v>67</v>
       </c>
-      <c r="D64" s="31" t="s">
+      <c r="D64" t="s">
         <v>739</v>
       </c>
-      <c r="E64" s="31" t="s">
+      <c r="E64" t="s">
         <v>16</v>
       </c>
-      <c r="F64" s="31">
-        <v>1</v>
-      </c>
-      <c r="G64" s="31"/>
-      <c r="H64" s="31">
+      <c r="F64">
+        <v>1</v>
+      </c>
+      <c r="H64">
         <v>575</v>
       </c>
-      <c r="I64" s="31"/>
-      <c r="J64" s="31"/>
-      <c r="K64" s="32">
+      <c r="K64" s="15">
         <f>MIN(Season4Data[[#This Row],[Brian]:[Spencer]])</f>
         <v>3</v>
       </c>
-      <c r="L64" s="33">
+      <c r="L64" s="29">
         <f>AVERAGE(Season4Data[[#This Row],[Brian]:[Spencer]])</f>
         <v>3.5</v>
       </c>
-      <c r="M64" s="31" t="b">
+      <c r="M64" t="b">
         <f>IF(COUNTIF(Season4Data[[#This Row],[Brian]:[Spencer]], Season3Data[[#This Row],[Best Guess]]) &gt; 1, TRUE, FALSE)</f>
         <v>1</v>
       </c>
-      <c r="N64" s="31"/>
-      <c r="O64" s="31">
-        <v>4</v>
-      </c>
-      <c r="P64" s="31"/>
-      <c r="Q64" s="31">
-        <v>3</v>
-      </c>
-      <c r="R64" s="31">
-        <v>3</v>
-      </c>
-      <c r="S64" s="31">
-        <v>4</v>
-      </c>
-      <c r="T64" s="31">
-        <v>4</v>
-      </c>
-      <c r="U64" s="31">
+      <c r="O64">
+        <v>4</v>
+      </c>
+      <c r="Q64">
+        <v>3</v>
+      </c>
+      <c r="R64">
+        <v>3</v>
+      </c>
+      <c r="S64">
+        <v>4</v>
+      </c>
+      <c r="T64">
+        <v>4</v>
+      </c>
+      <c r="U64">
         <v>3</v>
       </c>
       <c r="X64" t="s">
@@ -11517,57 +11512,52 @@
       <c r="A65" s="1">
         <v>45163</v>
       </c>
-      <c r="B65" s="31" t="s">
+      <c r="B65" t="s">
         <v>16</v>
       </c>
-      <c r="C65" s="31" t="s">
+      <c r="C65" t="s">
         <v>740</v>
       </c>
-      <c r="D65" s="31" t="s">
+      <c r="D65" t="s">
         <v>147</v>
       </c>
-      <c r="E65" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="F65" s="31">
-        <v>1</v>
-      </c>
-      <c r="G65" s="31"/>
-      <c r="H65" s="31">
+      <c r="E65" t="s">
+        <v>4</v>
+      </c>
+      <c r="F65">
+        <v>1</v>
+      </c>
+      <c r="H65">
         <v>372</v>
       </c>
-      <c r="I65" s="31"/>
-      <c r="J65" s="31"/>
-      <c r="K65" s="32">
+      <c r="K65" s="15">
         <f>MIN(Season4Data[[#This Row],[Brian]:[Spencer]])</f>
         <v>3</v>
       </c>
-      <c r="L65" s="33">
+      <c r="L65" s="29">
         <f>AVERAGE(Season4Data[[#This Row],[Brian]:[Spencer]])</f>
         <v>3.8333333333333335</v>
       </c>
-      <c r="M65" s="31" t="b">
+      <c r="M65" t="b">
         <f>IF(COUNTIF(Season4Data[[#This Row],[Brian]:[Spencer]], Season3Data[[#This Row],[Best Guess]]) &gt; 1, TRUE, FALSE)</f>
         <v>1</v>
       </c>
-      <c r="N65" s="31"/>
-      <c r="O65" s="31">
-        <v>3</v>
-      </c>
-      <c r="P65" s="31">
-        <v>5</v>
-      </c>
-      <c r="Q65" s="31">
-        <v>4</v>
-      </c>
-      <c r="R65" s="31">
-        <v>4</v>
-      </c>
-      <c r="S65" s="31">
-        <v>4</v>
-      </c>
-      <c r="T65" s="31"/>
-      <c r="U65" s="31">
+      <c r="O65">
+        <v>3</v>
+      </c>
+      <c r="P65">
+        <v>5</v>
+      </c>
+      <c r="Q65">
+        <v>4</v>
+      </c>
+      <c r="R65">
+        <v>4</v>
+      </c>
+      <c r="S65">
+        <v>4</v>
+      </c>
+      <c r="U65">
         <v>3</v>
       </c>
       <c r="X65" t="s">
@@ -11581,61 +11571,168 @@
       <c r="A66" s="1">
         <v>45164</v>
       </c>
-      <c r="B66" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="C66" s="31" t="s">
+      <c r="B66" t="s">
+        <v>4</v>
+      </c>
+      <c r="C66" t="s">
         <v>741</v>
       </c>
-      <c r="D66" s="31" t="s">
+      <c r="D66" t="s">
         <v>742</v>
       </c>
-      <c r="E66" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="F66" s="31">
-        <v>2</v>
-      </c>
-      <c r="G66" s="31"/>
-      <c r="H66" s="31">
-        <v>2</v>
-      </c>
-      <c r="I66" s="31"/>
-      <c r="J66" s="31"/>
-      <c r="K66" s="32">
+      <c r="E66" t="s">
+        <v>4</v>
+      </c>
+      <c r="F66">
+        <v>2</v>
+      </c>
+      <c r="H66">
+        <v>2</v>
+      </c>
+      <c r="K66" s="15">
         <f>MIN(Season4Data[[#This Row],[Brian]:[Spencer]])</f>
         <v>2</v>
       </c>
-      <c r="L66" s="33">
+      <c r="L66" s="29">
         <f>AVERAGE(Season4Data[[#This Row],[Brian]:[Spencer]])</f>
         <v>2.3333333333333335</v>
       </c>
-      <c r="M66" s="31" t="b">
+      <c r="M66" t="b">
         <f>IF(COUNTIF(Season4Data[[#This Row],[Brian]:[Spencer]], Season3Data[[#This Row],[Best Guess]]) &gt; 1, TRUE, FALSE)</f>
         <v>1</v>
       </c>
-      <c r="N66" s="31"/>
-      <c r="O66" s="31">
-        <v>2</v>
-      </c>
-      <c r="P66" s="31"/>
-      <c r="Q66" s="31">
-        <v>2</v>
-      </c>
-      <c r="R66" s="31">
-        <v>3</v>
-      </c>
-      <c r="S66" s="31">
-        <v>2</v>
-      </c>
-      <c r="T66" s="31">
-        <v>2</v>
-      </c>
-      <c r="U66" s="31">
-        <v>3</v>
+      <c r="O66">
+        <v>2</v>
+      </c>
+      <c r="Q66">
+        <v>2</v>
+      </c>
+      <c r="R66">
+        <v>3</v>
+      </c>
+      <c r="S66">
+        <v>2</v>
+      </c>
+      <c r="T66">
+        <v>2</v>
+      </c>
+      <c r="U66">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A67" s="1">
+        <v>45165</v>
+      </c>
+      <c r="B67" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="C67" s="32" t="s">
+        <v>743</v>
+      </c>
+      <c r="D67" s="32" t="s">
+        <v>744</v>
+      </c>
+      <c r="E67" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="F67" s="32">
+        <v>1</v>
+      </c>
+      <c r="G67" s="32"/>
+      <c r="H67" s="32">
+        <v>2101</v>
+      </c>
+      <c r="I67" s="32"/>
+      <c r="J67" s="32"/>
+      <c r="K67" s="33">
+        <f>MIN(Season4Data[[#This Row],[Brian]:[Spencer]])</f>
+        <v>3</v>
+      </c>
+      <c r="L67" s="34">
+        <f>AVERAGE(Season4Data[[#This Row],[Brian]:[Spencer]])</f>
+        <v>4.8</v>
+      </c>
+      <c r="M67" s="32" t="b">
+        <f>IF(COUNTIF(Season4Data[[#This Row],[Brian]:[Spencer]], Season3Data[[#This Row],[Best Guess]]) &gt; 1, TRUE, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="N67" s="32"/>
+      <c r="O67" s="32">
+        <v>6</v>
+      </c>
+      <c r="P67" s="32"/>
+      <c r="Q67" s="32">
+        <v>3</v>
+      </c>
+      <c r="R67" s="32">
+        <v>5</v>
+      </c>
+      <c r="S67" s="32">
+        <v>5</v>
+      </c>
+      <c r="T67" s="32"/>
+      <c r="U67" s="32">
+        <v>5</v>
       </c>
     </row>
     <row r="68" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A68" s="1">
+        <v>45166</v>
+      </c>
+      <c r="B68" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C68" s="32" t="s">
+        <v>153</v>
+      </c>
+      <c r="D68" s="32" t="s">
+        <v>745</v>
+      </c>
+      <c r="E68" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="F68" s="32">
+        <v>1</v>
+      </c>
+      <c r="G68" s="32"/>
+      <c r="H68" s="32">
+        <v>142</v>
+      </c>
+      <c r="I68" s="32"/>
+      <c r="J68" s="32"/>
+      <c r="K68" s="33">
+        <f>MIN(Season4Data[[#This Row],[Brian]:[Spencer]])</f>
+        <v>3</v>
+      </c>
+      <c r="L68" s="34">
+        <f>AVERAGE(Season4Data[[#This Row],[Brian]:[Spencer]])</f>
+        <v>3.8333333333333335</v>
+      </c>
+      <c r="M68" s="32" t="b">
+        <f>IF(COUNTIF(Season4Data[[#This Row],[Brian]:[Spencer]], Season3Data[[#This Row],[Best Guess]]) &gt; 1, TRUE, FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="N68" s="32"/>
+      <c r="O68" s="32">
+        <v>3</v>
+      </c>
+      <c r="P68" s="32"/>
+      <c r="Q68" s="32">
+        <v>3</v>
+      </c>
+      <c r="R68" s="32">
+        <v>4</v>
+      </c>
+      <c r="S68" s="32">
+        <v>3</v>
+      </c>
+      <c r="T68" s="32">
+        <v>4</v>
+      </c>
+      <c r="U68" s="32">
+        <v>6</v>
+      </c>
       <c r="X68" s="26" t="s">
         <v>376</v>
       </c>
@@ -11986,7 +12083,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="O2:U66">
+  <conditionalFormatting sqref="O2:U68">
     <cfRule type="containsBlanks" dxfId="138" priority="1">
       <formula>LEN(TRIM(O2))=0</formula>
     </cfRule>

</xml_diff>